<commit_message>
lock versions to the latest releases
</commit_message>
<xml_diff>
--- a/projects/template_lhs_discrete_continuous.xlsx
+++ b/projects/template_lhs_discrete_continuous.xlsx
@@ -2011,13 +2011,13 @@
     <t>Total Site Energy</t>
   </si>
   <si>
-    <t>1.5.4</t>
-  </si>
-  <si>
     <t>Choose which OpenStudio Server Version to Use.  Do NOT change this unless advised. Note that this is not the OpenStudio version.  See mappings here: http://developer.nrel.gov/downloads/buildings/openstudio/rsrc/amis_v2.json</t>
   </si>
   <si>
     <t xml:space="preserve"> - Worker Only - </t>
+  </si>
+  <si>
+    <t>1.5.6</t>
   </si>
 </sst>
 </file>
@@ -5453,7 +5453,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5511,10 +5511,10 @@
         <v>482</v>
       </c>
       <c r="B5" s="29" t="s">
+        <v>658</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>656</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="46" customHeight="1">
@@ -16462,7 +16462,7 @@
         <v>621</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="33" customFormat="1">
@@ -16476,7 +16476,7 @@
         <v>623</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="33" customFormat="1">

</xml_diff>

<commit_message>
update spreadsheets with ptacs
</commit_message>
<xml_diff>
--- a/projects/template_lhs_discrete_continuous.xlsx
+++ b/projects/template_lhs_discrete_continuous.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="562" activeTab="3"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="562" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="669">
   <si>
     <t>type</t>
   </si>
@@ -1687,9 +1687,6 @@
     <t>Set Hot Water Loop Temperature</t>
   </si>
   <si>
-    <t>Total Electricity</t>
-  </si>
-  <si>
     <t>epsilonGradient</t>
   </si>
   <si>
@@ -1846,9 +1843,6 @@
     <t>positive integer (if individual, total simulations is this times each variable)</t>
   </si>
   <si>
-    <t>Total Natural Gas</t>
-  </si>
-  <si>
     <t>m3.large</t>
   </si>
   <si>
@@ -1966,12 +1960,6 @@
     <t>discrete_uncertain</t>
   </si>
   <si>
-    <t>Total Source Energy</t>
-  </si>
-  <si>
-    <t>Total Site Energy</t>
-  </si>
-  <si>
     <t>Choose which OpenStudio Server Version to Use.  Do NOT change this unless advised. Note that this is not the OpenStudio version.  See mappings here: http://developer.nrel.gov/downloads/buildings/openstudio/rsrc/amis_v2.json</t>
   </si>
   <si>
@@ -2027,6 +2015,39 @@
   </si>
   <si>
     <t>standard_report_legacy.total_source_energy</t>
+  </si>
+  <si>
+    <t>Taxonomy Identifier</t>
+  </si>
+  <si>
+    <t>Machine Name thats Link to Dencity Taxonomy</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Total Site Energy Intensity</t>
+  </si>
+  <si>
+    <t>total_site_energy_intensity</t>
+  </si>
+  <si>
+    <t>Total Source Energy Intensity</t>
+  </si>
+  <si>
+    <t>total_source_energy_intensity</t>
+  </si>
+  <si>
+    <t>Total Natural Gas Intensity</t>
+  </si>
+  <si>
+    <t>total_natural_gas_intensity</t>
+  </si>
+  <si>
+    <t>Total Electricity Intensity</t>
+  </si>
+  <si>
+    <t>total_electricity_intensity</t>
   </si>
 </sst>
 </file>
@@ -5585,8 +5606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5622,7 +5643,7 @@
         <v>441</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>442</v>
@@ -5644,10 +5665,10 @@
         <v>477</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="46" customHeight="1">
@@ -5655,7 +5676,7 @@
         <v>478</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>480</v>
@@ -5666,7 +5687,7 @@
         <v>447</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C7" s="37" t="str">
         <f>VLOOKUP($B7,instance_defs,2,FALSE)&amp;VLOOKUP($B7,instance_defs,4,FALSE)</f>
@@ -5677,7 +5698,7 @@
         <v>$0.14/hour</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28">
@@ -5709,7 +5730,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="37"/>
       <c r="E9" s="2" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="12" customFormat="1">
@@ -5726,7 +5747,7 @@
         <v>42</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>479</v>
@@ -5770,7 +5791,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5789,7 +5810,7 @@
         <v>474</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>442</v>
@@ -5800,7 +5821,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -5825,13 +5846,13 @@
         <v>456</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>463</v>
@@ -5861,14 +5882,14 @@
       </c>
       <c r="B25" s="29">
         <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C25" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D25" s="40">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -6029,7 +6050,7 @@
         <v>31</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28">
@@ -6054,13 +6075,13 @@
         <v>34</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>455</v>
@@ -6074,11 +6095,11 @@
         <v>36</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -6114,7 +6135,7 @@
   <dimension ref="A1:Y91"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6184,10 +6205,10 @@
         <v>39</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -6233,7 +6254,7 @@
         <v>9</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>484</v>
@@ -6364,7 +6385,7 @@
         <v>68</v>
       </c>
       <c r="H8" s="34">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="3">
@@ -6587,7 +6608,7 @@
         <v>23</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>79</v>
@@ -6596,7 +6617,7 @@
         <v>68</v>
       </c>
       <c r="H17" s="34">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="34">
@@ -6656,7 +6677,7 @@
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>263</v>
@@ -6686,7 +6707,7 @@
       <c r="O19" s="33"/>
       <c r="P19" s="33"/>
       <c r="Q19" s="33" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="20" spans="1:18" s="34" customFormat="1" ht="15">
@@ -6813,7 +6834,7 @@
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>263</v>
@@ -6823,7 +6844,7 @@
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I24" s="17"/>
       <c r="J24" s="33">
@@ -6838,13 +6859,13 @@
       <c r="M24" s="33"/>
       <c r="N24" s="33"/>
       <c r="O24" s="33" t="s">
+        <v>634</v>
+      </c>
+      <c r="P24" s="33" t="s">
         <v>636</v>
       </c>
-      <c r="P24" s="33" t="s">
+      <c r="Q24" s="33" t="s">
         <v>638</v>
-      </c>
-      <c r="Q24" s="33" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="34" customFormat="1" ht="15">
@@ -7017,7 +7038,7 @@
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="17" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I31" s="17" t="s">
         <v>88</v>
@@ -7975,18 +7996,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="2" max="3" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="34" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.5" style="34" customWidth="1"/>
     <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
@@ -7995,65 +8015,69 @@
     <col min="10" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
+    <row r="1" spans="1:12" s="34" customFormat="1" ht="18">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="5"/>
+      <c r="G1" s="7"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="15">
-      <c r="A2" s="8" t="s">
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" s="14" customFormat="1" ht="45">
+      <c r="A2" s="14" t="s">
         <v>467</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="14" t="s">
+        <v>658</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>468</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="14" t="s">
+        <v>644</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>645</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>646</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>647</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>648</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>647</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>649</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>650</v>
-      </c>
-      <c r="I2" s="8" t="s">
+    </row>
+    <row r="3" spans="1:12" s="14" customFormat="1" ht="45">
+      <c r="A3" s="14" t="s">
         <v>651</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="B3" s="14" t="s">
+        <v>659</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>653</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
         <v>652</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="14" customFormat="1" ht="30">
-      <c r="A3" s="14" t="s">
-        <v>655</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>657</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10" t="s">
-        <v>656</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>469</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>469</v>
@@ -8062,139 +8086,160 @@
         <v>469</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>653</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="34" customFormat="1">
+        <v>469</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>649</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>650</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="34" customFormat="1">
       <c r="A4" s="33" t="s">
-        <v>601</v>
+        <v>661</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="C4" s="33" t="s">
+        <v>656</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>476</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="E4" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="33" t="b">
+      <c r="F4" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="33" t="b">
-        <v>0</v>
-      </c>
       <c r="G4" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="35"/>
+        <v>1</v>
+      </c>
+      <c r="H4" s="33" t="b">
+        <v>0</v>
+      </c>
       <c r="I4" s="33"/>
       <c r="J4" s="33"/>
-    </row>
-    <row r="5" spans="1:10" s="34" customFormat="1">
+      <c r="K4" s="33"/>
+    </row>
+    <row r="5" spans="1:12" s="34" customFormat="1">
       <c r="A5" s="33" t="s">
-        <v>548</v>
+        <v>663</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>659</v>
+        <v>664</v>
       </c>
       <c r="C5" s="33" t="s">
+        <v>657</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>476</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="E5" s="33" t="s">
         <v>68</v>
-      </c>
-      <c r="E5" s="33" t="b">
-        <v>1</v>
       </c>
       <c r="F5" s="33" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="35"/>
+        <v>1</v>
+      </c>
+      <c r="H5" s="33" t="b">
+        <v>0</v>
+      </c>
       <c r="I5" s="33"/>
       <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>642</v>
-      </c>
-      <c r="B6" t="s">
-        <v>660</v>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+    </row>
+    <row r="6" spans="1:12" s="34" customFormat="1">
+      <c r="A6" s="33" t="s">
+        <v>665</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>666</v>
       </c>
       <c r="C6" s="33" t="s">
+        <v>654</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>476</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="E6" s="33" t="s">
         <v>68</v>
-      </c>
-      <c r="E6" s="33" t="b">
-        <v>1</v>
       </c>
       <c r="F6" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="G6" t="b">
+      <c r="G6" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>641</v>
+      <c r="H6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+    </row>
+    <row r="7" spans="1:12" s="34" customFormat="1">
+      <c r="A7" s="33" t="s">
+        <v>667</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>661</v>
+        <v>668</v>
       </c>
       <c r="C7" s="33" t="s">
+        <v>655</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>476</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="E7" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="33" t="b">
+      <c r="F7" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="b">
+      <c r="G7" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="H7" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="35"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="J8"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:12">
       <c r="J9"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:12">
       <c r="J10"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:12">
       <c r="J11"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:12">
       <c r="J12"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:12">
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:12">
       <c r="J14"/>
     </row>
-    <row r="15" spans="1:10" customFormat="1">
+    <row r="15" spans="1:12" customFormat="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -8205,7 +8250,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:10" customFormat="1">
+    <row r="16" spans="1:12" customFormat="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -16502,72 +16547,72 @@
     </row>
     <row r="2" spans="1:21" s="33" customFormat="1">
       <c r="A2" s="33" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>450</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="33" customFormat="1">
       <c r="A3" s="33" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>451</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="33" customFormat="1">
       <c r="A4" s="33" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>452</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="33" customFormat="1">
       <c r="A5" s="33" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B5" s="33" t="s">
         <v>450</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="33" customFormat="1">
       <c r="A6" s="33" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>451</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="33" customFormat="1">
@@ -16578,52 +16623,52 @@
         <v>452</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="33" customFormat="1">
       <c r="A8" s="33" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>452</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="33" customFormat="1">
       <c r="A9" s="33" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>453</v>
       </c>
       <c r="C9" s="33" t="s">
+        <v>615</v>
+      </c>
+      <c r="D9" s="33" t="s">
         <v>617</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C11" s="18" t="s">
+        <v>564</v>
+      </c>
+      <c r="E11" t="s">
         <v>565</v>
       </c>
-      <c r="E11" t="s">
-        <v>566</v>
-      </c>
       <c r="G11" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -16634,7 +16679,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G12" t="s">
         <v>473</v>
@@ -16648,66 +16693,66 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="33" customFormat="1"/>
     <row r="16" spans="1:21">
       <c r="A16" t="s">
+        <v>558</v>
+      </c>
+      <c r="C16" t="s">
         <v>559</v>
-      </c>
-      <c r="C16" t="s">
-        <v>560</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L16" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="O16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="R16" s="33" t="s">
+        <v>562</v>
+      </c>
+      <c r="U16" s="33" t="s">
         <v>563</v>
-      </c>
-      <c r="U16" s="33" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F17" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G17" t="s">
         <v>462</v>
       </c>
       <c r="H17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J17" s="32">
         <v>0.01</v>
       </c>
       <c r="K17" s="34" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="M17">
         <v>30</v>
       </c>
       <c r="N17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="O17" t="s">
         <v>4</v>
@@ -16716,7 +16761,7 @@
         <v>30</v>
       </c>
       <c r="Q17" s="33" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -16730,229 +16775,229 @@
         <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J18" s="32">
         <v>0.01</v>
       </c>
       <c r="K18" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L18" s="34" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="M18">
         <v>5</v>
       </c>
       <c r="N18" s="33" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="O18" s="34" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="P18">
         <v>3</v>
       </c>
       <c r="Q18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="J19" s="32">
         <v>45036000000000</v>
       </c>
       <c r="K19" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="M19">
         <v>2</v>
       </c>
       <c r="N19" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="O19" s="34" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="P19">
         <v>0.85</v>
       </c>
       <c r="Q19" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="J20">
         <v>100</v>
       </c>
       <c r="K20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L20" t="s">
+        <v>591</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20" t="s">
         <v>592</v>
       </c>
-      <c r="M20">
-        <v>2</v>
-      </c>
-      <c r="N20" t="s">
-        <v>593</v>
-      </c>
       <c r="O20" s="34" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="P20">
         <v>2</v>
       </c>
       <c r="Q20" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I21" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="J21" s="34" t="s">
         <v>550</v>
       </c>
-      <c r="J21" s="34" t="s">
-        <v>551</v>
-      </c>
       <c r="L21" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="M21" s="32">
         <v>0.01</v>
       </c>
       <c r="N21" s="34" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="O21" s="34" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="P21">
         <v>2</v>
       </c>
       <c r="Q21" s="33" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="J22" s="34">
         <v>2</v>
       </c>
       <c r="K22" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="M22" s="32">
         <v>0.01</v>
       </c>
       <c r="N22" s="34" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="O22" s="34" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="P22">
         <v>0.8</v>
       </c>
       <c r="Q22" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M23" s="32">
         <v>0.01</v>
       </c>
       <c r="N23" s="33" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="O23" s="34" t="s">
+        <v>549</v>
+      </c>
+      <c r="P23" s="34" t="s">
         <v>550</v>
-      </c>
-      <c r="P23" s="34" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="L24" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="M24" s="32">
         <v>45036000000000</v>
       </c>
       <c r="N24" s="33" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="O24" s="34" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="P24" s="34">
         <v>2</v>
       </c>
       <c r="Q24" s="33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="L25" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="M25" s="33">
         <v>100</v>
       </c>
       <c r="N25" s="33" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="L26" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="M26" s="34" t="s">
         <v>550</v>
-      </c>
-      <c r="M26" s="34" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="L27" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="M27" s="34">
         <v>2</v>
       </c>
       <c r="N27" s="33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaning up files that are not to be released
</commit_message>
<xml_diff>
--- a/projects/template_lhs_discrete_continuous.xlsx
+++ b/projects/template_lhs_discrete_continuous.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="27640" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19840" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -1986,9 +1986,6 @@
     <t>standard_report_legacy.total_electricity</t>
   </si>
   <si>
-    <t>0.3.3</t>
-  </si>
-  <si>
     <t>Parameter Short Display Name</t>
   </si>
   <si>
@@ -2263,6 +2260,9 @@
   </si>
   <si>
     <t>South Projection Factor</t>
+  </si>
+  <si>
+    <t>0.3.5</t>
   </si>
 </sst>
 </file>
@@ -5791,8 +5791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5830,7 +5830,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>648</v>
+        <v>740</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>437</v>
@@ -5852,7 +5852,7 @@
         <v>471</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>618</v>
@@ -5874,7 +5874,7 @@
         <v>442</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C7" s="24" t="str">
         <f>VLOOKUP($B7,instance_defs,5,FALSE)</f>
@@ -5924,7 +5924,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="24" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E9" s="24" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
@@ -5949,7 +5949,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>473</v>
@@ -5960,7 +5960,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>619</v>
@@ -6264,7 +6264,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="2" customFormat="1" ht="28">
@@ -6290,13 +6290,13 @@
         <v>32</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>450</v>
@@ -6351,7 +6351,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z98"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -6468,7 +6470,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>11</v>
@@ -6614,7 +6616,7 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E6" s="42" t="s">
         <v>46</v>
@@ -6966,7 +6968,7 @@
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="42" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>75</v>
@@ -7052,7 +7054,7 @@
       </c>
       <c r="C17" s="46"/>
       <c r="D17" s="46" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E17" s="46" t="s">
         <v>258</v>
@@ -7082,7 +7084,7 @@
       <c r="P17" s="42"/>
       <c r="Q17" s="42"/>
       <c r="R17" s="42" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="S17" s="42"/>
       <c r="T17" s="42"/>
@@ -7252,7 +7254,7 @@
       </c>
       <c r="C22" s="46"/>
       <c r="D22" s="46" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E22" s="46" t="s">
         <v>258</v>
@@ -7275,16 +7277,18 @@
       <c r="M22" s="46">
         <v>50</v>
       </c>
-      <c r="N22" s="42"/>
+      <c r="N22" s="42">
+        <v>10</v>
+      </c>
       <c r="O22" s="42"/>
       <c r="P22" s="42" t="s">
+        <v>737</v>
+      </c>
+      <c r="Q22" s="42" t="s">
         <v>738</v>
       </c>
-      <c r="Q22" s="42" t="s">
-        <v>739</v>
-      </c>
       <c r="R22" s="42" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="S22" s="42"/>
       <c r="T22" s="42"/>
@@ -7454,7 +7458,7 @@
       </c>
       <c r="C27" s="46"/>
       <c r="D27" s="46" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E27" s="46" t="s">
         <v>77</v>
@@ -7618,7 +7622,7 @@
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="46" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>77</v>
@@ -7715,7 +7719,7 @@
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="10" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>84</v>
@@ -7782,13 +7786,13 @@
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="42" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>172</v>
       </c>
       <c r="F35" s="42" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G35" s="42" t="s">
         <v>64</v>
@@ -7922,7 +7926,7 @@
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
@@ -9719,7 +9723,7 @@
         <v>461</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>622</v>
@@ -9758,7 +9762,7 @@
         <v>629</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>630</v>
@@ -9797,7 +9801,7 @@
         <v>636</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>637</v>
@@ -9830,7 +9834,7 @@
         <v>639</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>640</v>
@@ -9863,7 +9867,7 @@
         <v>642</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>643</v>
@@ -9896,7 +9900,7 @@
         <v>645</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>646</v>
@@ -9926,15 +9930,15 @@
     </row>
     <row r="8" spans="1:13" s="23" customFormat="1">
       <c r="A8" s="15" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>64</v>
@@ -9955,15 +9959,15 @@
     </row>
     <row r="9" spans="1:13" s="23" customFormat="1">
       <c r="A9" s="15" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>64</v>
@@ -9984,15 +9988,15 @@
     </row>
     <row r="10" spans="1:13" s="23" customFormat="1">
       <c r="A10" s="15" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>64</v>
@@ -10013,15 +10017,15 @@
     </row>
     <row r="11" spans="1:13" s="23" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>64</v>
@@ -10042,12 +10046,12 @@
     </row>
     <row r="12" spans="1:13" s="23" customFormat="1">
       <c r="A12" s="15" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>470</v>
@@ -10071,12 +10075,12 @@
     </row>
     <row r="13" spans="1:13" s="23" customFormat="1">
       <c r="A13" s="15" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>470</v>
@@ -10100,12 +10104,12 @@
     </row>
     <row r="14" spans="1:13" s="23" customFormat="1">
       <c r="A14" s="15" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>470</v>
@@ -10129,12 +10133,12 @@
     </row>
     <row r="15" spans="1:13" s="23" customFormat="1">
       <c r="A15" s="15" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>470</v>
@@ -10158,12 +10162,12 @@
     </row>
     <row r="16" spans="1:13" s="23" customFormat="1">
       <c r="A16" s="15" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>470</v>
@@ -10187,12 +10191,12 @@
     </row>
     <row r="17" spans="1:13" s="22" customFormat="1">
       <c r="A17" s="15" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>470</v>
@@ -10216,12 +10220,12 @@
     </row>
     <row r="18" spans="1:13" s="22" customFormat="1">
       <c r="A18" s="15" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>470</v>
@@ -10245,12 +10249,12 @@
     </row>
     <row r="19" spans="1:13" s="22" customFormat="1">
       <c r="A19" s="15" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>470</v>
@@ -10274,12 +10278,12 @@
     </row>
     <row r="20" spans="1:13" s="22" customFormat="1">
       <c r="A20" s="15" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>470</v>
@@ -10303,12 +10307,12 @@
     </row>
     <row r="21" spans="1:13" s="22" customFormat="1">
       <c r="A21" s="15" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>470</v>
@@ -10332,12 +10336,12 @@
     </row>
     <row r="22" spans="1:13" s="22" customFormat="1">
       <c r="A22" s="15" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>470</v>
@@ -10361,12 +10365,12 @@
     </row>
     <row r="23" spans="1:13" s="23" customFormat="1">
       <c r="A23" s="15" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>470</v>
@@ -10390,12 +10394,12 @@
     </row>
     <row r="24" spans="1:13" s="23" customFormat="1">
       <c r="A24" s="15" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>470</v>
@@ -10419,12 +10423,12 @@
     </row>
     <row r="25" spans="1:13" s="23" customFormat="1">
       <c r="A25" s="15" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>470</v>
@@ -10448,15 +10452,15 @@
     </row>
     <row r="26" spans="1:13" s="23" customFormat="1">
       <c r="A26" s="15" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
+        <v>712</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>713</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>714</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>64</v>
@@ -18943,7 +18947,7 @@
         <v>439</v>
       </c>
       <c r="D1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -18951,19 +18955,19 @@
     </row>
     <row r="2" spans="1:7" s="22" customFormat="1">
       <c r="A2" s="22" t="s">
+        <v>651</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>652</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>653</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>654</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>655</v>
-      </c>
       <c r="E2" s="22" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="22" customFormat="1">
@@ -18977,10 +18981,10 @@
         <v>594</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="22" customFormat="1">
@@ -18994,10 +18998,10 @@
         <v>596</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="22" customFormat="1">
@@ -19011,44 +19015,44 @@
         <v>598</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="22" customFormat="1">
       <c r="A6" s="22" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>446</v>
       </c>
       <c r="C6" s="22" t="s">
+        <v>659</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>660</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>661</v>
-      </c>
       <c r="E6" s="22" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="22" customFormat="1">
       <c r="A7" s="22" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>447</v>
       </c>
       <c r="C7" s="22" t="s">
+        <v>662</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>663</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>664</v>
-      </c>
       <c r="E7" s="22" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1">
@@ -19062,10 +19066,10 @@
         <v>600</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="22" customFormat="1">
@@ -19079,10 +19083,10 @@
         <v>602</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -19096,10 +19100,10 @@
         <v>603</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1">
@@ -19113,10 +19117,10 @@
         <v>605</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="22" customFormat="1">
@@ -19124,16 +19128,16 @@
         <v>606</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>607</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="22" customFormat="1"/>

</xml_diff>

<commit_message>
updated spreadsheets and aws gem
</commit_message>
<xml_diff>
--- a/projects/template_lhs_discrete_continuous.xlsx
+++ b/projects/template_lhs_discrete_continuous.xlsx
@@ -2214,9 +2214,6 @@
     <t>discrete_uncertain</t>
   </si>
   <si>
-    <t>1.8.0-pre12</t>
-  </si>
-  <si>
     <t>South WWR</t>
   </si>
   <si>
@@ -2263,6 +2260,9 @@
   </si>
   <si>
     <t>0.3.5</t>
+  </si>
+  <si>
+    <t>1.8.0-rc2</t>
   </si>
 </sst>
 </file>
@@ -2424,8 +2424,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1481">
+  <cellStyleXfs count="1485">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4009,7 +4013,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1481">
+  <cellStyles count="1485">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4750,6 +4754,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1476" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1478" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1484" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5490,6 +5496,8 @@
     <cellStyle name="Hyperlink" xfId="1475" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1477" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1483" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5792,7 +5800,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5830,7 +5838,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>437</v>
@@ -5852,7 +5860,7 @@
         <v>471</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>724</v>
+        <v>740</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>618</v>
@@ -5897,7 +5905,7 @@
         <v>443</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C8" s="24" t="str">
         <f>VLOOKUP($B8,instance_defs,5,FALSE)</f>
@@ -5905,11 +5913,11 @@
       </c>
       <c r="D8" s="24" t="str">
         <f>VLOOKUP($B8,instance_defs,2,FALSE)&amp;" with "&amp;VLOOKUP($B8,instance_defs,4,FALSE)</f>
-        <v>32 Cores with 320 GB</v>
+        <v>16 Cores with 160 GB</v>
       </c>
       <c r="E8" s="24" t="str">
         <f>VLOOKUP($B8,instance_defs,3,FALSE)</f>
-        <v>$1.68/hour</v>
+        <v>$0.84/hour</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>444</v>
@@ -5928,7 +5936,7 @@
       </c>
       <c r="E9" s="24" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$2.17/hour</v>
+        <v>$1.33/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>609</v>
@@ -5949,7 +5957,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>473</v>
@@ -5960,7 +5968,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>619</v>
@@ -6264,7 +6272,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="2" customFormat="1" ht="28">
@@ -6290,13 +6298,13 @@
         <v>32</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>450</v>
@@ -6616,7 +6624,7 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E6" s="42" t="s">
         <v>46</v>
@@ -6968,7 +6976,7 @@
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="42" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>75</v>
@@ -7054,7 +7062,7 @@
       </c>
       <c r="C17" s="46"/>
       <c r="D17" s="46" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E17" s="46" t="s">
         <v>258</v>
@@ -7084,7 +7092,7 @@
       <c r="P17" s="42"/>
       <c r="Q17" s="42"/>
       <c r="R17" s="42" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="S17" s="42"/>
       <c r="T17" s="42"/>
@@ -7254,7 +7262,7 @@
       </c>
       <c r="C22" s="46"/>
       <c r="D22" s="46" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E22" s="46" t="s">
         <v>258</v>
@@ -7282,10 +7290,10 @@
       </c>
       <c r="O22" s="42"/>
       <c r="P22" s="42" t="s">
+        <v>736</v>
+      </c>
+      <c r="Q22" s="42" t="s">
         <v>737</v>
-      </c>
-      <c r="Q22" s="42" t="s">
-        <v>738</v>
       </c>
       <c r="R22" s="42" t="s">
         <v>723</v>
@@ -7458,7 +7466,7 @@
       </c>
       <c r="C27" s="46"/>
       <c r="D27" s="46" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E27" s="46" t="s">
         <v>77</v>
@@ -7622,7 +7630,7 @@
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="46" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>77</v>
@@ -7786,7 +7794,7 @@
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="42" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>172</v>
@@ -18923,7 +18931,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
use new aws and analysis gem
</commit_message>
<xml_diff>
--- a/projects/template_lhs_discrete_continuous.xlsx
+++ b/projects/template_lhs_discrete_continuous.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19840" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="27640" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2331" uniqueCount="743">
   <si>
     <t>type</t>
   </si>
@@ -2016,24 +2016,6 @@
     <t>80 GB</t>
   </si>
   <si>
-    <t>m2.2xlarge</t>
-  </si>
-  <si>
-    <t>$0.49/hour</t>
-  </si>
-  <si>
-    <t>850 GB</t>
-  </si>
-  <si>
-    <t>m2.4xlarge</t>
-  </si>
-  <si>
-    <t>$0.98/hour</t>
-  </si>
-  <si>
-    <t>840 GB</t>
-  </si>
-  <si>
     <t>16 GB</t>
   </si>
   <si>
@@ -2055,12 +2037,6 @@
     <t>Recommended for Server if large analysis because of storage</t>
   </si>
   <si>
-    <t>Worker Only</t>
-  </si>
-  <si>
-    <t>Worker Only - Recommended for Worker</t>
-  </si>
-  <si>
     <t>Storage</t>
   </si>
   <si>
@@ -2259,10 +2235,40 @@
     <t>South Projection Factor</t>
   </si>
   <si>
-    <t>0.3.5</t>
-  </si>
-  <si>
-    <t>1.8.0-rc2</t>
+    <t>1.8.0</t>
+  </si>
+  <si>
+    <t>AWS Tag</t>
+  </si>
+  <si>
+    <t>org=5500</t>
+  </si>
+  <si>
+    <t>Add extra tags to your instances (key=value). Add another line if you need another tag.</t>
+  </si>
+  <si>
+    <t>0.3.6</t>
+  </si>
+  <si>
+    <t>Recommended for worker</t>
+  </si>
+  <si>
+    <t>Can be used as worker</t>
+  </si>
+  <si>
+    <t>i2.2xlarge</t>
+  </si>
+  <si>
+    <t>i2.xlarge</t>
+  </si>
+  <si>
+    <t>$0.85/hour</t>
+  </si>
+  <si>
+    <t>800 GB</t>
+  </si>
+  <si>
+    <t>$1.71/hour</t>
   </si>
 </sst>
 </file>
@@ -2424,8 +2430,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1485">
+  <cellStyleXfs count="1515">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4013,7 +4049,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1485">
+  <cellStyles count="1515">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4756,6 +4792,21 @@
     <cellStyle name="Followed Hyperlink" xfId="1480" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1482" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1514" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5498,6 +5549,21 @@
     <cellStyle name="Hyperlink" xfId="1479" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1481" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1513" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5797,10 +5863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5838,7 +5904,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>437</v>
@@ -5860,7 +5926,7 @@
         <v>471</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>740</v>
+        <v>731</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>618</v>
@@ -5877,24 +5943,24 @@
         <v>474</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>442</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>658</v>
+        <v>595</v>
       </c>
       <c r="C7" s="24" t="str">
         <f>VLOOKUP($B7,instance_defs,5,FALSE)</f>
-        <v>Recommended for Server if large analysis because of storage</v>
+        <v>Recommended for Server</v>
       </c>
       <c r="D7" s="24" t="str">
         <f>VLOOKUP($B7,instance_defs,2,FALSE)&amp;" with "&amp;VLOOKUP($B7,instance_defs,4,FALSE)</f>
-        <v>4 Cores with 850 GB</v>
+        <v>4 Cores with 40 GB</v>
       </c>
       <c r="E7" s="24" t="str">
         <f>VLOOKUP($B7,instance_defs,3,FALSE)</f>
-        <v>$0.49/hour</v>
+        <v>$0.28/hour</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>610</v>
@@ -5905,19 +5971,19 @@
         <v>443</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>604</v>
+        <v>440</v>
       </c>
       <c r="C8" s="24" t="str">
         <f>VLOOKUP($B8,instance_defs,5,FALSE)</f>
-        <v>Worker Only - Recommended for Worker</v>
+        <v>Recommended for worker</v>
       </c>
       <c r="D8" s="24" t="str">
         <f>VLOOKUP($B8,instance_defs,2,FALSE)&amp;" with "&amp;VLOOKUP($B8,instance_defs,4,FALSE)</f>
-        <v>16 Cores with 160 GB</v>
+        <v>8 Cores with 80 GB</v>
       </c>
       <c r="E8" s="24" t="str">
         <f>VLOOKUP($B8,instance_defs,3,FALSE)</f>
-        <v>$0.84/hour</v>
+        <v>$0.42/hour</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>444</v>
@@ -5932,54 +5998,57 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="24" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="E9" s="24" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$1.33/hour</v>
+        <v>$0.7/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="7" customFormat="1">
-      <c r="A11" s="6" t="s">
+    <row r="10" spans="1:6" s="23" customFormat="1" ht="28">
+      <c r="A10" s="23" t="s">
+        <v>732</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>733</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="2" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="7" customFormat="1">
+      <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>726</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>473</v>
-      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>727</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>619</v>
+        <v>718</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>452</v>
+        <v>719</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>619</v>
@@ -5987,358 +6056,369 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="B15" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>437</v>
+        <v>26</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>452</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="B16" s="16" t="b">
+        <v>464</v>
+      </c>
+      <c r="B16" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>611</v>
+      <c r="F16" s="1" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>467</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>437</v>
+        <v>465</v>
+      </c>
+      <c r="B17" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>547</v>
+        <v>467</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" ht="42">
-      <c r="A20" s="6" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>547</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B21" s="19" t="s">
         <v>612</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="8" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="8" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B22" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="23" customFormat="1">
-      <c r="B22" s="18"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" ht="42">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:6" s="23" customFormat="1">
+      <c r="B23" s="18"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A24" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B24" s="19" t="s">
         <v>615</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>613</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>614</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="8" t="s">
+      <c r="E24" s="6"/>
+      <c r="F24" s="8" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
+    <row r="25" spans="1:6">
+      <c r="A25" s="23" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
         <v>Sample Method</v>
       </c>
-      <c r="B24" s="18" t="str">
-        <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
+      <c r="B25" s="18" t="str">
+        <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
         <v>all_variables</v>
       </c>
-      <c r="C24" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
+      <c r="C25" s="25" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v>individual_variables / all_variables</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D25" s="27" t="s">
         <v>454</v>
       </c>
-      <c r="E24" s="23"/>
-    </row>
-    <row r="25" spans="1:6" ht="28">
-      <c r="A25" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" spans="1:6" ht="28">
+      <c r="A26" s="23" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
         <v>Number of Samples</v>
       </c>
-      <c r="B25" s="18">
-        <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
+      <c r="B26" s="18">
+        <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
         <v>30</v>
       </c>
-      <c r="C25" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
+      <c r="C26" s="25" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D26" s="27">
         <v>30</v>
       </c>
-      <c r="E25" s="23"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
+      <c r="E26" s="23"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="23" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
         <v/>
       </c>
-      <c r="B26" s="18" t="str">
-        <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
+      <c r="B27" s="18" t="str">
+        <f>IF(D27&lt;&gt;"",D27,IF(LEN(INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
         <v/>
       </c>
-      <c r="C26" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
+      <c r="C27" s="25" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v/>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="23"/>
-    </row>
-    <row r="27" spans="1:6" s="23" customFormat="1">
-      <c r="A27" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v/>
-      </c>
-      <c r="B27" s="18" t="str">
-        <f>IF(D27&lt;&gt;"",D27,IF(LEN(INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v/>
-      </c>
-      <c r="C27" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v/>
-      </c>
       <c r="D27" s="27"/>
+      <c r="E27" s="23"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1">
       <c r="A28" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
         <v/>
       </c>
       <c r="B28" s="18" t="str">
-        <f>IF(D28&lt;&gt;"",D28,IF(LEN(INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
+        <f>IF(D28&lt;&gt;"",D28,IF(LEN(INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
         <v/>
       </c>
       <c r="C28" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v/>
       </c>
       <c r="D28" s="27"/>
     </row>
     <row r="29" spans="1:6" s="23" customFormat="1">
       <c r="A29" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
         <v/>
       </c>
       <c r="B29" s="18" t="str">
-        <f>IF(D29&lt;&gt;"",D29,IF(LEN(INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
+        <f>IF(D29&lt;&gt;"",D29,IF(LEN(INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
         <v/>
       </c>
       <c r="C29" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v/>
       </c>
       <c r="D29" s="27"/>
     </row>
     <row r="30" spans="1:6" s="23" customFormat="1">
       <c r="A30" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
         <v/>
       </c>
       <c r="B30" s="18" t="str">
-        <f>IF(D30&lt;&gt;"",D30,IF(LEN(INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
+        <f>IF(D30&lt;&gt;"",D30,IF(LEN(INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
         <v/>
       </c>
       <c r="C30" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v/>
       </c>
       <c r="D30" s="27"/>
     </row>
     <row r="31" spans="1:6" s="23" customFormat="1">
       <c r="A31" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
         <v/>
       </c>
       <c r="B31" s="18" t="str">
-        <f>IF(D31&lt;&gt;"",D31,IF(LEN(INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
+        <f>IF(D31&lt;&gt;"",D31,IF(LEN(INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
         <v/>
       </c>
       <c r="C31" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v/>
       </c>
       <c r="D31" s="27"/>
     </row>
     <row r="32" spans="1:6" s="23" customFormat="1">
       <c r="A32" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
         <v/>
       </c>
       <c r="B32" s="18" t="str">
-        <f>IF(D32&lt;&gt;"",D32,IF(LEN(INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
+        <f>IF(D32&lt;&gt;"",D32,IF(LEN(INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
         <v/>
       </c>
       <c r="C32" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v/>
       </c>
       <c r="D32" s="27"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" s="23" customFormat="1">
       <c r="A33" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
         <v/>
       </c>
       <c r="B33" s="18" t="str">
-        <f>IF(D33&lt;&gt;"",D33,IF(LEN(INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
+        <f>IF(D33&lt;&gt;"",D33,IF(LEN(INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
         <v/>
       </c>
       <c r="C33" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v/>
       </c>
       <c r="D33" s="27"/>
-      <c r="E33" s="23"/>
-    </row>
-    <row r="34" spans="1:6" s="23" customFormat="1">
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="23" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
         <v/>
       </c>
       <c r="B34" s="18" t="str">
-        <f>IF(D34&lt;&gt;"",D34,IF(LEN(INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
+        <f>IF(D34&lt;&gt;"",D34,IF(LEN(INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
         <v/>
       </c>
       <c r="C34" s="25" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v/>
       </c>
       <c r="D34" s="27"/>
+      <c r="E34" s="23"/>
     </row>
     <row r="35" spans="1:6" s="23" customFormat="1">
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" ht="28">
-      <c r="A36" s="6" t="s">
+      <c r="A35" s="23" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-2))</f>
+        <v/>
+      </c>
+      <c r="B35" s="18" t="str">
+        <f>IF(D35&lt;&gt;"",D35,IF(LEN(INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
+        <v/>
+      </c>
+      <c r="C35" s="25" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
+        <v/>
+      </c>
+      <c r="D35" s="27"/>
+    </row>
+    <row r="36" spans="1:6" s="23" customFormat="1">
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A37" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B37" s="19" t="s">
         <v>620</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="1" t="s">
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="26" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" ht="28">
-      <c r="A39" s="6" t="s">
+      <c r="B38" s="26" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A40" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B40" s="19" t="s">
         <v>455</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>620</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="8" t="s">
+      <c r="E40" s="6"/>
+      <c r="F40" s="8" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28">
-      <c r="A40" s="23" t="s">
+    <row r="41" spans="1:6" ht="28">
+      <c r="A41" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="17" t="s">
-        <v>729</v>
-      </c>
-      <c r="C40" s="14" t="s">
+      <c r="B41" s="17" t="s">
+        <v>721</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>730</v>
-      </c>
-      <c r="F40" s="2" t="s">
+      <c r="D41" s="14" t="s">
+        <v>722</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="2" customFormat="1" ht="56">
-      <c r="A42" s="6" t="s">
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="56">
+      <c r="A43" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B43" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>621</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="8" t="s">
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="8" t="s">
         <v>616</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
       <formula1>AnalysisType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B17">
       <formula1>TrueFalse</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
       <formula1>Workflow</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
       <formula1>simulate_data_point</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B7:B8">
@@ -6624,7 +6704,7 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="E6" s="42" t="s">
         <v>46</v>
@@ -6976,7 +7056,7 @@
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="42" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>75</v>
@@ -7062,7 +7142,7 @@
       </c>
       <c r="C17" s="46"/>
       <c r="D17" s="46" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="E17" s="46" t="s">
         <v>258</v>
@@ -7092,7 +7172,7 @@
       <c r="P17" s="42"/>
       <c r="Q17" s="42"/>
       <c r="R17" s="42" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="S17" s="42"/>
       <c r="T17" s="42"/>
@@ -7262,7 +7342,7 @@
       </c>
       <c r="C22" s="46"/>
       <c r="D22" s="46" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
       <c r="E22" s="46" t="s">
         <v>258</v>
@@ -7290,13 +7370,13 @@
       </c>
       <c r="O22" s="42"/>
       <c r="P22" s="42" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="Q22" s="42" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="R22" s="42" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
       <c r="S22" s="42"/>
       <c r="T22" s="42"/>
@@ -7466,7 +7546,7 @@
       </c>
       <c r="C27" s="46"/>
       <c r="D27" s="46" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="E27" s="46" t="s">
         <v>77</v>
@@ -7630,7 +7710,7 @@
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="46" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>77</v>
@@ -7727,7 +7807,7 @@
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="10" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>84</v>
@@ -7794,13 +7874,13 @@
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="42" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>172</v>
       </c>
       <c r="F35" s="42" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
       <c r="G35" s="42" t="s">
         <v>64</v>
@@ -7934,7 +8014,7 @@
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
@@ -9809,7 +9889,7 @@
         <v>636</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>637</v>
@@ -9842,7 +9922,7 @@
         <v>639</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>640</v>
@@ -9875,7 +9955,7 @@
         <v>642</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>643</v>
@@ -9908,7 +9988,7 @@
         <v>645</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>646</v>
@@ -9938,15 +10018,15 @@
     </row>
     <row r="8" spans="1:13" s="23" customFormat="1">
       <c r="A8" s="15" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>64</v>
@@ -9967,15 +10047,15 @@
     </row>
     <row r="9" spans="1:13" s="23" customFormat="1">
       <c r="A9" s="15" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>64</v>
@@ -9996,15 +10076,15 @@
     </row>
     <row r="10" spans="1:13" s="23" customFormat="1">
       <c r="A10" s="15" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>64</v>
@@ -10025,15 +10105,15 @@
     </row>
     <row r="11" spans="1:13" s="23" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>64</v>
@@ -10054,12 +10134,12 @@
     </row>
     <row r="12" spans="1:13" s="23" customFormat="1">
       <c r="A12" s="15" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>470</v>
@@ -10083,12 +10163,12 @@
     </row>
     <row r="13" spans="1:13" s="23" customFormat="1">
       <c r="A13" s="15" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>470</v>
@@ -10112,12 +10192,12 @@
     </row>
     <row r="14" spans="1:13" s="23" customFormat="1">
       <c r="A14" s="15" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>470</v>
@@ -10141,12 +10221,12 @@
     </row>
     <row r="15" spans="1:13" s="23" customFormat="1">
       <c r="A15" s="15" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>470</v>
@@ -10170,12 +10250,12 @@
     </row>
     <row r="16" spans="1:13" s="23" customFormat="1">
       <c r="A16" s="15" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>470</v>
@@ -10199,12 +10279,12 @@
     </row>
     <row r="17" spans="1:13" s="22" customFormat="1">
       <c r="A17" s="15" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>470</v>
@@ -10228,12 +10308,12 @@
     </row>
     <row r="18" spans="1:13" s="22" customFormat="1">
       <c r="A18" s="15" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>470</v>
@@ -10257,12 +10337,12 @@
     </row>
     <row r="19" spans="1:13" s="22" customFormat="1">
       <c r="A19" s="15" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>470</v>
@@ -10286,12 +10366,12 @@
     </row>
     <row r="20" spans="1:13" s="22" customFormat="1">
       <c r="A20" s="15" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>470</v>
@@ -10315,12 +10395,12 @@
     </row>
     <row r="21" spans="1:13" s="22" customFormat="1">
       <c r="A21" s="15" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>470</v>
@@ -10344,12 +10424,12 @@
     </row>
     <row r="22" spans="1:13" s="22" customFormat="1">
       <c r="A22" s="15" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>470</v>
@@ -10373,12 +10453,12 @@
     </row>
     <row r="23" spans="1:13" s="23" customFormat="1">
       <c r="A23" s="15" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>470</v>
@@ -10402,12 +10482,12 @@
     </row>
     <row r="24" spans="1:13" s="23" customFormat="1">
       <c r="A24" s="15" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>470</v>
@@ -10431,12 +10511,12 @@
     </row>
     <row r="25" spans="1:13" s="23" customFormat="1">
       <c r="A25" s="15" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>470</v>
@@ -10460,15 +10540,15 @@
     </row>
     <row r="26" spans="1:13" s="23" customFormat="1">
       <c r="A26" s="15" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>64</v>
@@ -18931,7 +19011,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -18955,14 +19035,14 @@
         <v>439</v>
       </c>
       <c r="D1" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="22" customFormat="1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="29" t="s">
         <v>651</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -18975,11 +19055,11 @@
         <v>654</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="22" customFormat="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="29" t="s">
         <v>593</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -18992,11 +19072,11 @@
         <v>655</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="22" customFormat="1">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="29" t="s">
         <v>595</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -19009,11 +19089,11 @@
         <v>656</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="22" customFormat="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="29" t="s">
         <v>597</v>
       </c>
       <c r="B5" s="22" t="s">
@@ -19026,126 +19106,126 @@
         <v>657</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="22" customFormat="1">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="29" t="s">
+        <v>599</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>600</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>658</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="E6" s="22" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="22" customFormat="1">
+      <c r="A7" s="29" t="s">
+        <v>601</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>446</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C7" s="22" t="s">
+        <v>602</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>656</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="22" customFormat="1">
+      <c r="A8" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>447</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>603</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>657</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="22" customFormat="1">
+      <c r="A9" s="29" t="s">
+        <v>604</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>659</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="E9" s="22" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="29" t="s">
+        <v>606</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>660</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="22" customFormat="1">
-      <c r="A7" s="22" t="s">
+      <c r="C10" s="22" t="s">
+        <v>607</v>
+      </c>
+      <c r="D10" s="22" t="s">
         <v>661</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="E10" s="22" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="22" customFormat="1">
+      <c r="A11" s="29" t="s">
+        <v>739</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>446</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>740</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>741</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="22" customFormat="1">
+      <c r="A12" s="29" t="s">
+        <v>738</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>447</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>662</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>663</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="22" customFormat="1">
-      <c r="A8" s="22" t="s">
-        <v>599</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>445</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>600</v>
-      </c>
-      <c r="D8" s="22" t="s">
+      <c r="C12" s="22" t="s">
+        <v>742</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>741</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>664</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="22" customFormat="1">
-      <c r="A9" s="22" t="s">
-        <v>601</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>446</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>602</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>656</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="22" t="s">
-        <v>440</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>447</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>603</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>657</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="22" customFormat="1">
-      <c r="A11" s="22" t="s">
-        <v>604</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>448</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>605</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>665</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="22" customFormat="1">
-      <c r="A12" s="22" t="s">
-        <v>606</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>666</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>607</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>667</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="22" customFormat="1"/>

</xml_diff>

<commit_message>
add local measures and add more measures to lhs example
</commit_message>
<xml_diff>
--- a/projects/template_lhs_discrete_continuous.xlsx
+++ b/projects/template_lhs_discrete_continuous.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="27640" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2331" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="746">
   <si>
     <t>type</t>
   </si>
@@ -2160,9 +2160,6 @@
     <t>$</t>
   </si>
   <si>
-    <t>West PF</t>
-  </si>
-  <si>
     <t>Site EUI</t>
   </si>
   <si>
@@ -2269,6 +2266,18 @@
   </si>
   <si>
     <t>$1.71/hour</t>
+  </si>
+  <si>
+    <t>West WWR</t>
+  </si>
+  <si>
+    <t>South PF</t>
+  </si>
+  <si>
+    <t>East PF</t>
+  </si>
+  <si>
+    <t>East Projection Factor</t>
   </si>
 </sst>
 </file>
@@ -2430,8 +2439,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1515">
+  <cellStyleXfs count="1523">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4049,7 +4066,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1515">
+  <cellStyles count="1523">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4807,6 +4824,10 @@
     <cellStyle name="Followed Hyperlink" xfId="1510" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1512" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1522" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5564,6 +5585,10 @@
     <cellStyle name="Hyperlink" xfId="1509" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1511" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1521" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5866,7 +5891,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5904,7 +5929,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>437</v>
@@ -5926,7 +5951,7 @@
         <v>471</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>618</v>
@@ -5971,7 +5996,7 @@
         <v>443</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>440</v>
+        <v>604</v>
       </c>
       <c r="C8" s="24" t="str">
         <f>VLOOKUP($B8,instance_defs,5,FALSE)</f>
@@ -5979,11 +6004,11 @@
       </c>
       <c r="D8" s="24" t="str">
         <f>VLOOKUP($B8,instance_defs,2,FALSE)&amp;" with "&amp;VLOOKUP($B8,instance_defs,4,FALSE)</f>
-        <v>8 Cores with 80 GB</v>
+        <v>16 Cores with 160 GB</v>
       </c>
       <c r="E8" s="24" t="str">
         <f>VLOOKUP($B8,instance_defs,3,FALSE)</f>
-        <v>$0.42/hour</v>
+        <v>$0.84/hour</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>444</v>
@@ -6002,7 +6027,7 @@
       </c>
       <c r="E9" s="24" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$0.7/hour</v>
+        <v>$1.12/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>609</v>
@@ -6010,16 +6035,16 @@
     </row>
     <row r="10" spans="1:6" s="23" customFormat="1" ht="28">
       <c r="A10" s="23" t="s">
+        <v>731</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>732</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>733</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1">
@@ -6037,7 +6062,7 @@
         <v>39</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>473</v>
@@ -6048,7 +6073,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>619</v>
@@ -6179,14 +6204,14 @@
       </c>
       <c r="B26" s="18">
         <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="C26" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D26" s="27">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="E26" s="23"/>
     </row>
@@ -6352,7 +6377,7 @@
         <v>29</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="28">
@@ -6378,13 +6403,13 @@
         <v>32</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>450</v>
@@ -6437,10 +6462,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z98"/>
+  <dimension ref="A1:Z97"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6704,7 +6729,7 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E6" s="42" t="s">
         <v>46</v>
@@ -7056,7 +7081,7 @@
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="42" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>75</v>
@@ -7142,7 +7167,7 @@
       </c>
       <c r="C17" s="46"/>
       <c r="D17" s="46" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E17" s="46" t="s">
         <v>258</v>
@@ -7172,7 +7197,7 @@
       <c r="P17" s="42"/>
       <c r="Q17" s="42"/>
       <c r="R17" s="42" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="S17" s="42"/>
       <c r="T17" s="42"/>
@@ -7342,7 +7367,7 @@
       </c>
       <c r="C22" s="46"/>
       <c r="D22" s="46" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E22" s="46" t="s">
         <v>258</v>
@@ -7370,13 +7395,13 @@
       </c>
       <c r="O22" s="42"/>
       <c r="P22" s="42" t="s">
+        <v>727</v>
+      </c>
+      <c r="Q22" s="42" t="s">
         <v>728</v>
       </c>
-      <c r="Q22" s="42" t="s">
-        <v>729</v>
-      </c>
       <c r="R22" s="42" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="S22" s="42"/>
       <c r="T22" s="42"/>
@@ -7546,7 +7571,7 @@
       </c>
       <c r="C27" s="46"/>
       <c r="D27" s="46" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E27" s="46" t="s">
         <v>77</v>
@@ -7643,7 +7668,7 @@
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10" t="s">
-        <v>617</v>
+        <v>82</v>
       </c>
       <c r="J29" s="10" t="s">
         <v>84</v>
@@ -7710,7 +7735,7 @@
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="46" t="s">
-        <v>717</v>
+        <v>742</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>77</v>
@@ -7751,7 +7776,7 @@
       <c r="Y31" s="42"/>
       <c r="Z31" s="42"/>
     </row>
-    <row r="32" spans="1:26" s="22" customFormat="1" ht="15">
+    <row r="32" spans="1:26" s="29" customFormat="1" ht="15">
       <c r="A32" s="10"/>
       <c r="B32" s="10" t="s">
         <v>21</v>
@@ -7789,7 +7814,7 @@
       <c r="Y32" s="15"/>
       <c r="Z32" s="15"/>
     </row>
-    <row r="33" spans="1:26" s="29" customFormat="1" ht="15">
+    <row r="33" spans="1:26" s="22" customFormat="1" ht="15">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
         <v>21</v>
@@ -7807,7 +7832,7 @@
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="10" t="s">
-        <v>667</v>
+        <v>617</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>84</v>
@@ -7829,27 +7854,27 @@
       <c r="Y33" s="15"/>
       <c r="Z33" s="15"/>
     </row>
-    <row r="34" spans="1:26" s="28" customFormat="1">
-      <c r="A34" s="39" t="b">
+    <row r="34" spans="1:26" s="22" customFormat="1" ht="15">
+      <c r="A34" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="B34" s="39" t="s">
-        <v>169</v>
+      <c r="B34" s="45" t="s">
+        <v>383</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="D34" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="E34" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
       <c r="K34" s="39"/>
       <c r="L34" s="39"/>
       <c r="M34" s="39"/>
@@ -7867,46 +7892,44 @@
       <c r="Y34" s="39"/>
       <c r="Z34" s="39"/>
     </row>
-    <row r="35" spans="1:26" s="22" customFormat="1">
-      <c r="A35" s="42"/>
-      <c r="B35" s="42" t="s">
+    <row r="35" spans="1:26" s="22" customFormat="1" ht="15">
+      <c r="A35" s="46"/>
+      <c r="B35" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42" t="s">
-        <v>730</v>
-      </c>
-      <c r="E35" s="42" t="s">
-        <v>172</v>
-      </c>
-      <c r="F35" s="42" t="s">
-        <v>706</v>
-      </c>
-      <c r="G35" s="42" t="s">
+      <c r="C35" s="46"/>
+      <c r="D35" s="46" t="s">
+        <v>716</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="J35" s="42"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46">
+        <v>0.4</v>
+      </c>
+      <c r="J35" s="46"/>
       <c r="K35" s="42">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="L35" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="M35" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="N35" s="42">
-        <v>0.133333333</v>
-      </c>
-      <c r="O35" s="42"/>
+        <v>0.95</v>
+      </c>
+      <c r="M35" s="46">
+        <v>0.4</v>
+      </c>
+      <c r="N35" s="43">
+        <v>0.15</v>
+      </c>
+      <c r="O35" s="43"/>
       <c r="P35" s="42"/>
       <c r="Q35" s="42"/>
       <c r="R35" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S35" s="42"/>
       <c r="T35" s="42"/>
@@ -7917,29 +7940,27 @@
       <c r="Y35" s="42"/>
       <c r="Z35" s="42"/>
     </row>
-    <row r="36" spans="1:26" s="22" customFormat="1">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>84</v>
-      </c>
+    <row r="36" spans="1:26" s="22" customFormat="1" ht="15">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10">
+        <v>30</v>
+      </c>
+      <c r="J36" s="10"/>
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
@@ -7957,29 +7978,31 @@
       <c r="Y36" s="15"/>
       <c r="Z36" s="15"/>
     </row>
-    <row r="37" spans="1:26" s="22" customFormat="1">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
+    <row r="37" spans="1:26" s="29" customFormat="1" ht="15">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
@@ -7995,154 +8018,164 @@
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
     </row>
-    <row r="38" spans="1:26" s="29" customFormat="1">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15" t="s">
+    <row r="38" spans="1:26" s="28" customFormat="1">
+      <c r="A38" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="39"/>
+      <c r="P38" s="39"/>
+      <c r="Q38" s="39"/>
+      <c r="R38" s="39"/>
+      <c r="S38" s="39"/>
+      <c r="T38" s="39"/>
+      <c r="U38" s="39"/>
+      <c r="V38" s="39"/>
+      <c r="W38" s="39"/>
+      <c r="X38" s="39"/>
+      <c r="Y38" s="39"/>
+      <c r="Z38" s="39"/>
+    </row>
+    <row r="39" spans="1:26" s="22" customFormat="1">
+      <c r="A39" s="42"/>
+      <c r="B39" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42" t="s">
+        <v>729</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="F39" s="42" t="s">
+        <v>743</v>
+      </c>
+      <c r="G39" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42">
+        <v>0</v>
+      </c>
+      <c r="J39" s="42"/>
+      <c r="K39" s="42">
+        <v>0</v>
+      </c>
+      <c r="L39" s="42">
+        <v>1</v>
+      </c>
+      <c r="M39" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="N39" s="42">
+        <v>0.133333333</v>
+      </c>
+      <c r="O39" s="42"/>
+      <c r="P39" s="42"/>
+      <c r="Q39" s="42"/>
+      <c r="R39" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="S39" s="42"/>
+      <c r="T39" s="42"/>
+      <c r="U39" s="42"/>
+      <c r="V39" s="42"/>
+      <c r="W39" s="42"/>
+      <c r="X39" s="42"/>
+      <c r="Y39" s="42"/>
+      <c r="Z39" s="42"/>
+    </row>
+    <row r="40" spans="1:26" s="22" customFormat="1">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15" t="s">
-        <v>668</v>
-      </c>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
-      <c r="U38" s="15"/>
-      <c r="V38" s="15"/>
-      <c r="W38" s="15"/>
-      <c r="X38" s="15"/>
-      <c r="Y38" s="15"/>
-      <c r="Z38" s="15"/>
-    </row>
-    <row r="39" spans="1:26" s="28" customFormat="1" ht="15">
-      <c r="A39" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="B39" s="45" t="s">
-        <v>399</v>
-      </c>
-      <c r="C39" s="39" t="s">
-        <v>400</v>
-      </c>
-      <c r="D39" s="45" t="s">
-        <v>400</v>
-      </c>
-      <c r="E39" s="45" t="s">
-        <v>160</v>
-      </c>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="39"/>
-      <c r="N39" s="39"/>
-      <c r="O39" s="39"/>
-      <c r="P39" s="39"/>
-      <c r="Q39" s="39"/>
-      <c r="R39" s="39"/>
-      <c r="S39" s="39"/>
-      <c r="T39" s="39"/>
-      <c r="U39" s="39"/>
-      <c r="V39" s="39"/>
-      <c r="W39" s="39"/>
-      <c r="X39" s="39"/>
-      <c r="Y39" s="39"/>
-      <c r="Z39" s="39"/>
-    </row>
-    <row r="40" spans="1:26" s="22" customFormat="1" ht="15">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10"/>
-      <c r="T40" s="10"/>
-      <c r="U40" s="10"/>
-      <c r="V40" s="10"/>
-      <c r="W40" s="10"/>
-      <c r="X40" s="10"/>
-      <c r="Y40" s="10"/>
-      <c r="Z40" s="10"/>
-    </row>
-    <row r="41" spans="1:26" s="22" customFormat="1" ht="15">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10" t="s">
-        <v>433</v>
-      </c>
-      <c r="J41" s="10" t="s">
-        <v>434</v>
-      </c>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-      <c r="S41" s="10"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="J40" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15"/>
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="15"/>
+    </row>
+    <row r="41" spans="1:26" s="22" customFormat="1">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
       <c r="T41" s="15"/>
       <c r="U41" s="15"/>
       <c r="V41" s="15"/>
@@ -8151,19 +8184,29 @@
       <c r="Y41" s="15"/>
       <c r="Z41" s="15"/>
     </row>
-    <row r="42" spans="1:26" s="22" customFormat="1" ht="15">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
+    <row r="42" spans="1:26" s="29" customFormat="1">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15" t="s">
+        <v>668</v>
+      </c>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
       <c r="O42" s="15"/>
@@ -8179,75 +8222,119 @@
       <c r="Y42" s="15"/>
       <c r="Z42" s="15"/>
     </row>
-    <row r="43" spans="1:26" s="29" customFormat="1" ht="15">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="41"/>
-      <c r="Q43" s="41"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="15"/>
-      <c r="Z43" s="15"/>
-    </row>
-    <row r="44" spans="1:26" s="28" customFormat="1" ht="15">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="15"/>
-    </row>
-    <row r="45" spans="1:26" s="22" customFormat="1" ht="15">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="10"/>
+    <row r="43" spans="1:26" s="28" customFormat="1">
+      <c r="A43" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B43" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="E43" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="39"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="39"/>
+      <c r="O43" s="39"/>
+      <c r="P43" s="39"/>
+      <c r="Q43" s="39"/>
+      <c r="R43" s="39"/>
+      <c r="S43" s="39"/>
+      <c r="T43" s="39"/>
+      <c r="U43" s="39"/>
+      <c r="V43" s="39"/>
+      <c r="W43" s="39"/>
+      <c r="X43" s="39"/>
+      <c r="Y43" s="39"/>
+      <c r="Z43" s="39"/>
+    </row>
+    <row r="44" spans="1:26" s="22" customFormat="1">
+      <c r="A44" s="42"/>
+      <c r="B44" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42" t="s">
+        <v>745</v>
+      </c>
+      <c r="E44" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="F44" s="42" t="s">
+        <v>744</v>
+      </c>
+      <c r="G44" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42">
+        <v>0</v>
+      </c>
+      <c r="J44" s="42"/>
+      <c r="K44" s="42">
+        <v>0</v>
+      </c>
+      <c r="L44" s="42">
+        <v>1</v>
+      </c>
+      <c r="M44" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="N44" s="42">
+        <v>0.133333333</v>
+      </c>
+      <c r="O44" s="42"/>
+      <c r="P44" s="42"/>
+      <c r="Q44" s="42"/>
+      <c r="R44" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="S44" s="42"/>
+      <c r="T44" s="42"/>
+      <c r="U44" s="42"/>
+      <c r="V44" s="42"/>
+      <c r="W44" s="42"/>
+      <c r="X44" s="42"/>
+      <c r="Y44" s="42"/>
+      <c r="Z44" s="42"/>
+    </row>
+    <row r="45" spans="1:26" s="22" customFormat="1">
+      <c r="A45" s="15"/>
+      <c r="B45" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15" t="s">
+        <v>667</v>
+      </c>
+      <c r="J45" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
       <c r="O45" s="15"/>
@@ -8263,19 +8350,29 @@
       <c r="Y45" s="15"/>
       <c r="Z45" s="15"/>
     </row>
-    <row r="46" spans="1:26" s="22" customFormat="1" ht="15">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="10"/>
+    <row r="46" spans="1:26" s="22" customFormat="1">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
       <c r="O46" s="15"/>
@@ -8291,19 +8388,29 @@
       <c r="Y46" s="15"/>
       <c r="Z46" s="15"/>
     </row>
-    <row r="47" spans="1:26" s="22" customFormat="1" ht="15">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
+    <row r="47" spans="1:26" s="29" customFormat="1">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15" t="s">
+        <v>668</v>
+      </c>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
       <c r="O47" s="15"/>
@@ -8319,82 +8426,116 @@
       <c r="Y47" s="15"/>
       <c r="Z47" s="15"/>
     </row>
-    <row r="48" spans="1:26" s="29" customFormat="1" ht="15">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
-      <c r="T48" s="15"/>
-      <c r="U48" s="15"/>
-      <c r="V48" s="15"/>
-      <c r="W48" s="15"/>
-      <c r="X48" s="15"/>
-      <c r="Y48" s="15"/>
-      <c r="Z48" s="15"/>
+    <row r="48" spans="1:26" s="28" customFormat="1" ht="15">
+      <c r="A48" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="B48" s="45" t="s">
+        <v>399</v>
+      </c>
+      <c r="C48" s="39" t="s">
+        <v>400</v>
+      </c>
+      <c r="D48" s="45" t="s">
+        <v>400</v>
+      </c>
+      <c r="E48" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="39"/>
+      <c r="L48" s="39"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="39"/>
+      <c r="O48" s="39"/>
+      <c r="P48" s="39"/>
+      <c r="Q48" s="39"/>
+      <c r="R48" s="39"/>
+      <c r="S48" s="39"/>
+      <c r="T48" s="39"/>
+      <c r="U48" s="39"/>
+      <c r="V48" s="39"/>
+      <c r="W48" s="39"/>
+      <c r="X48" s="39"/>
+      <c r="Y48" s="39"/>
+      <c r="Z48" s="39"/>
     </row>
     <row r="49" spans="1:26" s="22" customFormat="1" ht="15">
       <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
+      <c r="B49" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
+      <c r="D49" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>402</v>
+      </c>
       <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
+      <c r="G49" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
+      <c r="I49" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>432</v>
+      </c>
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="15"/>
-      <c r="O49" s="15"/>
-      <c r="P49" s="15"/>
-      <c r="Q49" s="15"/>
-      <c r="R49" s="15"/>
-      <c r="S49" s="15"/>
-      <c r="T49" s="15"/>
-      <c r="U49" s="15"/>
-      <c r="V49" s="15"/>
-      <c r="W49" s="15"/>
-      <c r="X49" s="15"/>
-      <c r="Y49" s="15"/>
-      <c r="Z49" s="15"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="10"/>
+      <c r="R49" s="10"/>
+      <c r="S49" s="10"/>
+      <c r="T49" s="10"/>
+      <c r="U49" s="10"/>
+      <c r="V49" s="10"/>
+      <c r="W49" s="10"/>
+      <c r="X49" s="10"/>
+      <c r="Y49" s="10"/>
+      <c r="Z49" s="10"/>
     </row>
     <row r="50" spans="1:26" s="22" customFormat="1" ht="15">
       <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
+      <c r="B50" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
+      <c r="D50" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>404</v>
+      </c>
       <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
+      <c r="G50" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
+      <c r="I50" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>434</v>
+      </c>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
-      <c r="M50" s="15"/>
-      <c r="N50" s="15"/>
-      <c r="O50" s="15"/>
-      <c r="P50" s="15"/>
-      <c r="Q50" s="15"/>
-      <c r="R50" s="15"/>
-      <c r="S50" s="15"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10"/>
       <c r="T50" s="15"/>
       <c r="U50" s="15"/>
       <c r="V50" s="15"/>
@@ -8488,7 +8629,7 @@
       <c r="Z53" s="15"/>
     </row>
     <row r="54" spans="1:26" customFormat="1" ht="15">
-      <c r="A54" s="10"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -8515,8 +8656,8 @@
       <c r="Y54" s="15"/>
       <c r="Z54" s="15"/>
     </row>
-    <row r="55" spans="1:26" customFormat="1" ht="15">
-      <c r="A55" s="15"/>
+    <row r="55" spans="1:26" ht="15">
+      <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -8543,7 +8684,7 @@
       <c r="Y55" s="15"/>
       <c r="Z55" s="15"/>
     </row>
-    <row r="56" spans="1:26" ht="15">
+    <row r="56" spans="1:26" customFormat="1" ht="15">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -8556,11 +8697,11 @@
       <c r="J56" s="10"/>
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
-      <c r="M56" s="15"/>
-      <c r="N56" s="15"/>
-      <c r="O56" s="15"/>
-      <c r="P56" s="15"/>
-      <c r="Q56" s="15"/>
+      <c r="M56" s="41"/>
+      <c r="N56" s="41"/>
+      <c r="O56" s="41"/>
+      <c r="P56" s="41"/>
+      <c r="Q56" s="41"/>
       <c r="R56" s="15"/>
       <c r="S56" s="15"/>
       <c r="T56" s="15"/>
@@ -8571,8 +8712,8 @@
       <c r="Y56" s="15"/>
       <c r="Z56" s="15"/>
     </row>
-    <row r="57" spans="1:26" customFormat="1" ht="15">
-      <c r="A57" s="10"/>
+    <row r="57" spans="1:26" ht="15">
+      <c r="A57" s="15"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -8584,11 +8725,11 @@
       <c r="J57" s="10"/>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
-      <c r="M57" s="41"/>
-      <c r="N57" s="41"/>
-      <c r="O57" s="41"/>
-      <c r="P57" s="41"/>
-      <c r="Q57" s="41"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
       <c r="S57" s="15"/>
       <c r="T57" s="15"/>
@@ -8600,7 +8741,7 @@
       <c r="Z57" s="15"/>
     </row>
     <row r="58" spans="1:26" ht="15">
-      <c r="A58" s="15"/>
+      <c r="A58" s="10"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -8612,7 +8753,7 @@
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
-      <c r="M58" s="15"/>
+      <c r="M58" s="10"/>
       <c r="N58" s="15"/>
       <c r="O58" s="15"/>
       <c r="P58" s="15"/>
@@ -8640,11 +8781,11 @@
       <c r="J59" s="10"/>
       <c r="K59" s="10"/>
       <c r="L59" s="10"/>
-      <c r="M59" s="10"/>
-      <c r="N59" s="15"/>
-      <c r="O59" s="15"/>
-      <c r="P59" s="15"/>
-      <c r="Q59" s="15"/>
+      <c r="M59" s="41"/>
+      <c r="N59" s="41"/>
+      <c r="O59" s="41"/>
+      <c r="P59" s="41"/>
+      <c r="Q59" s="41"/>
       <c r="R59" s="15"/>
       <c r="S59" s="15"/>
       <c r="T59" s="15"/>
@@ -8656,7 +8797,7 @@
       <c r="Z59" s="15"/>
     </row>
     <row r="60" spans="1:26" ht="15">
-      <c r="A60" s="10"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -8668,11 +8809,11 @@
       <c r="J60" s="10"/>
       <c r="K60" s="10"/>
       <c r="L60" s="10"/>
-      <c r="M60" s="41"/>
-      <c r="N60" s="41"/>
-      <c r="O60" s="41"/>
-      <c r="P60" s="41"/>
-      <c r="Q60" s="41"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="15"/>
+      <c r="Q60" s="15"/>
       <c r="R60" s="15"/>
       <c r="S60" s="15"/>
       <c r="T60" s="15"/>
@@ -8684,7 +8825,7 @@
       <c r="Z60" s="15"/>
     </row>
     <row r="61" spans="1:26" ht="15">
-      <c r="A61" s="15"/>
+      <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -8696,7 +8837,7 @@
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
       <c r="L61" s="10"/>
-      <c r="M61" s="15"/>
+      <c r="M61" s="10"/>
       <c r="N61" s="15"/>
       <c r="O61" s="15"/>
       <c r="P61" s="15"/>
@@ -8724,11 +8865,11 @@
       <c r="J62" s="10"/>
       <c r="K62" s="10"/>
       <c r="L62" s="10"/>
-      <c r="M62" s="10"/>
-      <c r="N62" s="15"/>
-      <c r="O62" s="15"/>
-      <c r="P62" s="15"/>
-      <c r="Q62" s="15"/>
+      <c r="M62" s="41"/>
+      <c r="N62" s="41"/>
+      <c r="O62" s="41"/>
+      <c r="P62" s="41"/>
+      <c r="Q62" s="41"/>
       <c r="R62" s="15"/>
       <c r="S62" s="15"/>
       <c r="T62" s="15"/>
@@ -8740,7 +8881,7 @@
       <c r="Z62" s="15"/>
     </row>
     <row r="63" spans="1:26" ht="15">
-      <c r="A63" s="10"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -8752,11 +8893,11 @@
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
-      <c r="M63" s="41"/>
-      <c r="N63" s="41"/>
-      <c r="O63" s="41"/>
-      <c r="P63" s="41"/>
-      <c r="Q63" s="41"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="15"/>
       <c r="R63" s="15"/>
       <c r="S63" s="15"/>
       <c r="T63" s="15"/>
@@ -8768,7 +8909,7 @@
       <c r="Z63" s="15"/>
     </row>
     <row r="64" spans="1:26" ht="15">
-      <c r="A64" s="15"/>
+      <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
@@ -8780,7 +8921,7 @@
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
       <c r="L64" s="10"/>
-      <c r="M64" s="15"/>
+      <c r="M64" s="10"/>
       <c r="N64" s="15"/>
       <c r="O64" s="15"/>
       <c r="P64" s="15"/>
@@ -8808,11 +8949,11 @@
       <c r="J65" s="10"/>
       <c r="K65" s="10"/>
       <c r="L65" s="10"/>
-      <c r="M65" s="10"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="15"/>
-      <c r="P65" s="15"/>
-      <c r="Q65" s="15"/>
+      <c r="M65" s="41"/>
+      <c r="N65" s="41"/>
+      <c r="O65" s="41"/>
+      <c r="P65" s="41"/>
+      <c r="Q65" s="41"/>
       <c r="R65" s="15"/>
       <c r="S65" s="15"/>
       <c r="T65" s="15"/>
@@ -8824,7 +8965,7 @@
       <c r="Z65" s="15"/>
     </row>
     <row r="66" spans="1:26" ht="15">
-      <c r="A66" s="10"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
@@ -8836,11 +8977,11 @@
       <c r="J66" s="10"/>
       <c r="K66" s="10"/>
       <c r="L66" s="10"/>
-      <c r="M66" s="41"/>
-      <c r="N66" s="41"/>
-      <c r="O66" s="41"/>
-      <c r="P66" s="41"/>
-      <c r="Q66" s="41"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="O66" s="15"/>
+      <c r="P66" s="15"/>
+      <c r="Q66" s="15"/>
       <c r="R66" s="15"/>
       <c r="S66" s="15"/>
       <c r="T66" s="15"/>
@@ -8852,7 +8993,7 @@
       <c r="Z66" s="15"/>
     </row>
     <row r="67" spans="1:26" ht="15">
-      <c r="A67" s="15"/>
+      <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
@@ -8864,7 +9005,7 @@
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
       <c r="L67" s="10"/>
-      <c r="M67" s="15"/>
+      <c r="M67" s="10"/>
       <c r="N67" s="15"/>
       <c r="O67" s="15"/>
       <c r="P67" s="15"/>
@@ -8892,11 +9033,11 @@
       <c r="J68" s="10"/>
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
-      <c r="M68" s="10"/>
-      <c r="N68" s="15"/>
-      <c r="O68" s="15"/>
-      <c r="P68" s="15"/>
-      <c r="Q68" s="15"/>
+      <c r="M68" s="41"/>
+      <c r="N68" s="41"/>
+      <c r="O68" s="41"/>
+      <c r="P68" s="41"/>
+      <c r="Q68" s="41"/>
       <c r="R68" s="15"/>
       <c r="S68" s="15"/>
       <c r="T68" s="15"/>
@@ -8907,24 +9048,24 @@
       <c r="Y68" s="15"/>
       <c r="Z68" s="15"/>
     </row>
-    <row r="69" spans="1:26" ht="15">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10"/>
-      <c r="H69" s="10"/>
-      <c r="I69" s="10"/>
-      <c r="J69" s="10"/>
-      <c r="K69" s="10"/>
-      <c r="L69" s="10"/>
-      <c r="M69" s="41"/>
-      <c r="N69" s="41"/>
-      <c r="O69" s="41"/>
-      <c r="P69" s="41"/>
-      <c r="Q69" s="41"/>
+    <row r="69" spans="1:26">
+      <c r="A69" s="15"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="15"/>
+      <c r="P69" s="15"/>
+      <c r="Q69" s="15"/>
       <c r="R69" s="15"/>
       <c r="S69" s="15"/>
       <c r="T69" s="15"/>
@@ -9006,8 +9147,8 @@
       <c r="L72" s="15"/>
       <c r="M72" s="15"/>
       <c r="N72" s="15"/>
-      <c r="O72" s="15"/>
-      <c r="P72" s="15"/>
+      <c r="O72" s="41"/>
+      <c r="P72" s="41"/>
       <c r="Q72" s="15"/>
       <c r="R72" s="15"/>
       <c r="S72" s="15"/>
@@ -9034,8 +9175,8 @@
       <c r="L73" s="15"/>
       <c r="M73" s="15"/>
       <c r="N73" s="15"/>
-      <c r="O73" s="41"/>
-      <c r="P73" s="41"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
       <c r="Q73" s="15"/>
       <c r="R73" s="15"/>
       <c r="S73" s="15"/>
@@ -9159,7 +9300,7 @@
       <c r="Y77" s="15"/>
       <c r="Z77" s="15"/>
     </row>
-    <row r="78" spans="1:26">
+    <row r="78" spans="1:26" ht="15">
       <c r="A78" s="15"/>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
@@ -9173,9 +9314,9 @@
       <c r="K78" s="15"/>
       <c r="L78" s="15"/>
       <c r="M78" s="15"/>
-      <c r="N78" s="15"/>
-      <c r="O78" s="15"/>
-      <c r="P78" s="15"/>
+      <c r="N78" s="10"/>
+      <c r="O78" s="41"/>
+      <c r="P78" s="41"/>
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
       <c r="S78" s="15"/>
@@ -9187,7 +9328,7 @@
       <c r="Y78" s="15"/>
       <c r="Z78" s="15"/>
     </row>
-    <row r="79" spans="1:26" ht="15">
+    <row r="79" spans="1:26">
       <c r="A79" s="15"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
@@ -9201,9 +9342,9 @@
       <c r="K79" s="15"/>
       <c r="L79" s="15"/>
       <c r="M79" s="15"/>
-      <c r="N79" s="10"/>
-      <c r="O79" s="41"/>
-      <c r="P79" s="41"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15"/>
+      <c r="P79" s="15"/>
       <c r="Q79" s="15"/>
       <c r="R79" s="15"/>
       <c r="S79" s="15"/>
@@ -9355,8 +9496,8 @@
       <c r="Y84" s="15"/>
       <c r="Z84" s="15"/>
     </row>
-    <row r="85" spans="1:26">
-      <c r="A85" s="15"/>
+    <row r="85" spans="1:26" ht="15">
+      <c r="A85" s="10"/>
       <c r="B85" s="15"/>
       <c r="C85" s="15"/>
       <c r="D85" s="15"/>
@@ -9370,8 +9511,8 @@
       <c r="L85" s="15"/>
       <c r="M85" s="15"/>
       <c r="N85" s="15"/>
-      <c r="O85" s="15"/>
-      <c r="P85" s="15"/>
+      <c r="O85" s="41"/>
+      <c r="P85" s="41"/>
       <c r="Q85" s="15"/>
       <c r="R85" s="15"/>
       <c r="S85" s="15"/>
@@ -9383,8 +9524,8 @@
       <c r="Y85" s="15"/>
       <c r="Z85" s="15"/>
     </row>
-    <row r="86" spans="1:26" ht="15">
-      <c r="A86" s="10"/>
+    <row r="86" spans="1:26">
+      <c r="A86" s="15"/>
       <c r="B86" s="15"/>
       <c r="C86" s="15"/>
       <c r="D86" s="15"/>
@@ -9398,8 +9539,8 @@
       <c r="L86" s="15"/>
       <c r="M86" s="15"/>
       <c r="N86" s="15"/>
-      <c r="O86" s="41"/>
-      <c r="P86" s="41"/>
+      <c r="O86" s="15"/>
+      <c r="P86" s="15"/>
       <c r="Q86" s="15"/>
       <c r="R86" s="15"/>
       <c r="S86" s="15"/>
@@ -9426,8 +9567,8 @@
       <c r="L87" s="15"/>
       <c r="M87" s="15"/>
       <c r="N87" s="15"/>
-      <c r="O87" s="15"/>
-      <c r="P87" s="15"/>
+      <c r="O87" s="41"/>
+      <c r="P87" s="41"/>
       <c r="Q87" s="15"/>
       <c r="R87" s="15"/>
       <c r="S87" s="15"/>
@@ -9482,8 +9623,8 @@
       <c r="L89" s="15"/>
       <c r="M89" s="15"/>
       <c r="N89" s="15"/>
-      <c r="O89" s="41"/>
-      <c r="P89" s="41"/>
+      <c r="O89" s="15"/>
+      <c r="P89" s="15"/>
       <c r="Q89" s="15"/>
       <c r="R89" s="15"/>
       <c r="S89" s="15"/>
@@ -9510,8 +9651,8 @@
       <c r="L90" s="15"/>
       <c r="M90" s="15"/>
       <c r="N90" s="15"/>
-      <c r="O90" s="15"/>
-      <c r="P90" s="15"/>
+      <c r="O90" s="41"/>
+      <c r="P90" s="41"/>
       <c r="Q90" s="15"/>
       <c r="R90" s="15"/>
       <c r="S90" s="15"/>
@@ -9538,8 +9679,8 @@
       <c r="L91" s="15"/>
       <c r="M91" s="15"/>
       <c r="N91" s="15"/>
-      <c r="O91" s="41"/>
-      <c r="P91" s="41"/>
+      <c r="O91" s="15"/>
+      <c r="P91" s="15"/>
       <c r="Q91" s="15"/>
       <c r="R91" s="15"/>
       <c r="S91" s="15"/>
@@ -9566,8 +9707,8 @@
       <c r="L92" s="15"/>
       <c r="M92" s="15"/>
       <c r="N92" s="15"/>
-      <c r="O92" s="15"/>
-      <c r="P92" s="15"/>
+      <c r="O92" s="41"/>
+      <c r="P92" s="41"/>
       <c r="Q92" s="15"/>
       <c r="R92" s="15"/>
       <c r="S92" s="15"/>
@@ -9594,8 +9735,8 @@
       <c r="L93" s="15"/>
       <c r="M93" s="15"/>
       <c r="N93" s="15"/>
-      <c r="O93" s="41"/>
-      <c r="P93" s="41"/>
+      <c r="O93" s="15"/>
+      <c r="P93" s="15"/>
       <c r="Q93" s="15"/>
       <c r="R93" s="15"/>
       <c r="S93" s="15"/>
@@ -9622,8 +9763,8 @@
       <c r="L94" s="15"/>
       <c r="M94" s="15"/>
       <c r="N94" s="15"/>
-      <c r="O94" s="15"/>
-      <c r="P94" s="15"/>
+      <c r="O94" s="41"/>
+      <c r="P94" s="41"/>
       <c r="Q94" s="15"/>
       <c r="R94" s="15"/>
       <c r="S94" s="15"/>
@@ -9650,8 +9791,8 @@
       <c r="L95" s="15"/>
       <c r="M95" s="15"/>
       <c r="N95" s="15"/>
-      <c r="O95" s="41"/>
-      <c r="P95" s="41"/>
+      <c r="O95" s="15"/>
+      <c r="P95" s="15"/>
       <c r="Q95" s="15"/>
       <c r="R95" s="15"/>
       <c r="S95" s="15"/>
@@ -9678,8 +9819,8 @@
       <c r="L96" s="15"/>
       <c r="M96" s="15"/>
       <c r="N96" s="15"/>
-      <c r="O96" s="15"/>
-      <c r="P96" s="15"/>
+      <c r="O96" s="41"/>
+      <c r="P96" s="41"/>
       <c r="Q96" s="15"/>
       <c r="R96" s="15"/>
       <c r="S96" s="15"/>
@@ -9706,8 +9847,8 @@
       <c r="L97" s="15"/>
       <c r="M97" s="15"/>
       <c r="N97" s="15"/>
-      <c r="O97" s="41"/>
-      <c r="P97" s="41"/>
+      <c r="O97" s="15"/>
+      <c r="P97" s="15"/>
       <c r="Q97" s="15"/>
       <c r="R97" s="15"/>
       <c r="S97" s="15"/>
@@ -9718,34 +9859,6 @@
       <c r="X97" s="15"/>
       <c r="Y97" s="15"/>
       <c r="Z97" s="15"/>
-    </row>
-    <row r="98" spans="1:26">
-      <c r="A98" s="15"/>
-      <c r="B98" s="15"/>
-      <c r="C98" s="15"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="15"/>
-      <c r="F98" s="15"/>
-      <c r="G98" s="15"/>
-      <c r="H98" s="15"/>
-      <c r="I98" s="15"/>
-      <c r="J98" s="15"/>
-      <c r="K98" s="15"/>
-      <c r="L98" s="15"/>
-      <c r="M98" s="15"/>
-      <c r="N98" s="15"/>
-      <c r="O98" s="15"/>
-      <c r="P98" s="15"/>
-      <c r="Q98" s="15"/>
-      <c r="R98" s="15"/>
-      <c r="S98" s="15"/>
-      <c r="T98" s="15"/>
-      <c r="U98" s="15"/>
-      <c r="V98" s="15"/>
-      <c r="W98" s="15"/>
-      <c r="X98" s="15"/>
-      <c r="Y98" s="15"/>
-      <c r="Z98" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -9889,7 +10002,7 @@
         <v>636</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>637</v>
@@ -9922,7 +10035,7 @@
         <v>639</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>640</v>
@@ -9955,7 +10068,7 @@
         <v>642</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>643</v>
@@ -9988,7 +10101,7 @@
         <v>645</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>646</v>
@@ -10023,7 +10136,7 @@
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>670</v>
@@ -10052,7 +10165,7 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>670</v>
@@ -10081,7 +10194,7 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>670</v>
@@ -10110,7 +10223,7 @@
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>674</v>
@@ -19123,7 +19236,7 @@
         <v>658</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="22" customFormat="1">
@@ -19140,7 +19253,7 @@
         <v>656</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1">
@@ -19157,7 +19270,7 @@
         <v>657</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="22" customFormat="1">
@@ -19174,7 +19287,7 @@
         <v>659</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -19191,21 +19304,21 @@
         <v>661</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1">
       <c r="A11" s="29" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>446</v>
       </c>
       <c r="C11" s="22" t="s">
+        <v>739</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>740</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>741</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>664</v>
@@ -19213,16 +19326,16 @@
     </row>
     <row r="12" spans="1:7" s="22" customFormat="1">
       <c r="A12" s="29" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>447</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>664</v>

</xml_diff>

<commit_message>
update spreadsheet format to include worker inits
</commit_message>
<xml_diff>
--- a/projects/template_lhs_discrete_continuous.xlsx
+++ b/projects/template_lhs_discrete_continuous.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19840" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2387" uniqueCount="762">
   <si>
     <t>type</t>
   </si>
@@ -2244,9 +2244,6 @@
     <t>Add extra tags to your instances (key=value). Add another line if you need another tag.</t>
   </si>
   <si>
-    <t>0.3.6</t>
-  </si>
-  <si>
     <t>Recommended for worker</t>
   </si>
   <si>
@@ -2278,6 +2275,57 @@
   </si>
   <si>
     <t>East Projection Factor</t>
+  </si>
+  <si>
+    <t>Worker Initialization Scripts - Name</t>
+  </si>
+  <si>
+    <t>Path (relative or absolute) to local script)</t>
+  </si>
+  <si>
+    <t>Worker Finalization Scripts - Name</t>
+  </si>
+  <si>
+    <t>These scripts will be executed in this order on each worker node when it is initialized.  These can be used to download any analysis-wide files such as BCL data, utility data, etc. Name is arbitary, but a name must exist to include the line.</t>
+  </si>
+  <si>
+    <t>These scripts will be executed in this order on each worker node when it is finalized. Can be used to push all the results of the anlaysis to a specific location. Name is arbitary, but a name must exist to include the line.</t>
+  </si>
+  <si>
+    <t>Arguments (in the form of an array ["19837,"z",{b: 'something'}])</t>
+  </si>
+  <si>
+    <t>Example Worker Init Script</t>
+  </si>
+  <si>
+    <t>../worker_scripts/example_init_file.rb</t>
+  </si>
+  <si>
+    <t>Path (relative or absolute) to local script</t>
+  </si>
+  <si>
+    <t>["Argument 1", 2]</t>
+  </si>
+  <si>
+    <t>This is an example of configuring a worker initialization script.</t>
+  </si>
+  <si>
+    <t>Window to Wall Ratio South</t>
+  </si>
+  <si>
+    <t>Window to Wall Ratio West</t>
+  </si>
+  <si>
+    <t>Window to Wall Ratio East</t>
+  </si>
+  <si>
+    <t>Overhangs PF South</t>
+  </si>
+  <si>
+    <t>Overhangs PF East</t>
+  </si>
+  <si>
+    <t>0.3.7</t>
   </si>
 </sst>
 </file>
@@ -2439,8 +2487,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1523">
+  <cellStyleXfs count="1559">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4066,7 +4150,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1523">
+  <cellStyles count="1559">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4828,6 +4912,24 @@
     <cellStyle name="Followed Hyperlink" xfId="1518" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1520" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1558" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5589,6 +5691,24 @@
     <cellStyle name="Hyperlink" xfId="1517" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1519" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1557" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5888,11 +6008,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -5928,8 +6046,8 @@
       <c r="A3" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>734</v>
+      <c r="B3" s="44" t="s">
+        <v>761</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>437</v>
@@ -6204,14 +6322,14 @@
       </c>
       <c r="B26" s="18">
         <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>300</v>
+        <v>5</v>
       </c>
       <c r="C26" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D26" s="27">
-        <v>300</v>
+        <v>5</v>
       </c>
       <c r="E26" s="23"/>
     </row>
@@ -6429,6 +6547,62 @@
       <c r="E43" s="6"/>
       <c r="F43" s="8" t="s">
         <v>616</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="2" customFormat="1">
+      <c r="B44" s="25"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="46" spans="1:6" s="2" customFormat="1" ht="56">
+      <c r="A46" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>753</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="8" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="2" customFormat="1">
+      <c r="A47" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>752</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="7" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="23" customFormat="1">
+      <c r="B48" s="18"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A49" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="8" t="s">
+        <v>749</v>
       </c>
     </row>
   </sheetData>
@@ -6464,8 +6638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z97"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7126,7 +7300,7 @@
       <c r="A16" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="39" t="s">
         <v>255</v>
       </c>
       <c r="C16" s="39" t="s">
@@ -7326,7 +7500,7 @@
       <c r="A21" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="39" t="s">
         <v>265</v>
       </c>
       <c r="C21" s="39" t="s">
@@ -7530,8 +7704,8 @@
       <c r="A26" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="B26" s="45" t="s">
-        <v>383</v>
+      <c r="B26" s="39" t="s">
+        <v>756</v>
       </c>
       <c r="C26" s="39" t="s">
         <v>76</v>
@@ -7694,8 +7868,8 @@
       <c r="A30" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="B30" s="45" t="s">
-        <v>383</v>
+      <c r="B30" s="39" t="s">
+        <v>757</v>
       </c>
       <c r="C30" s="39" t="s">
         <v>76</v>
@@ -7735,7 +7909,7 @@
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="46" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>77</v>
@@ -7858,8 +8032,8 @@
       <c r="A34" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="B34" s="45" t="s">
-        <v>383</v>
+      <c r="B34" s="39" t="s">
+        <v>758</v>
       </c>
       <c r="C34" s="39" t="s">
         <v>76</v>
@@ -8023,7 +8197,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>169</v>
+        <v>759</v>
       </c>
       <c r="C38" s="39" t="s">
         <v>170</v>
@@ -8069,7 +8243,7 @@
         <v>172</v>
       </c>
       <c r="F39" s="42" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="G39" s="42" t="s">
         <v>64</v>
@@ -8227,7 +8401,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>169</v>
+        <v>760</v>
       </c>
       <c r="C43" s="39" t="s">
         <v>170</v>
@@ -8267,13 +8441,13 @@
       </c>
       <c r="C44" s="42"/>
       <c r="D44" s="42" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E44" s="42" t="s">
         <v>172</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="G44" s="42" t="s">
         <v>64</v>
@@ -9881,7 +10055,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9889,7 +10063,7 @@
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
@@ -10145,7 +10319,7 @@
         <v>64</v>
       </c>
       <c r="G8" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="15" t="b">
         <v>1</v>
@@ -10174,7 +10348,7 @@
         <v>64</v>
       </c>
       <c r="G9" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="15" t="b">
         <v>1</v>
@@ -10203,7 +10377,7 @@
         <v>64</v>
       </c>
       <c r="G10" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="15" t="b">
         <v>1</v>
@@ -19236,7 +19410,7 @@
         <v>658</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="22" customFormat="1">
@@ -19253,7 +19427,7 @@
         <v>656</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1">
@@ -19270,7 +19444,7 @@
         <v>657</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="22" customFormat="1">
@@ -19287,7 +19461,7 @@
         <v>659</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -19304,21 +19478,21 @@
         <v>661</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1">
       <c r="A11" s="29" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>446</v>
       </c>
       <c r="C11" s="22" t="s">
+        <v>738</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>739</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>740</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>664</v>
@@ -19326,16 +19500,16 @@
     </row>
     <row r="12" spans="1:7" s="22" customFormat="1">
       <c r="A12" s="29" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>447</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>664</v>

</xml_diff>

<commit_message>
update to new images with energyplus 8.2
</commit_message>
<xml_diff>
--- a/projects/template_lhs_discrete_continuous.xlsx
+++ b/projects/template_lhs_discrete_continuous.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19840" tabRatio="562"/>
@@ -2232,9 +2232,6 @@
     <t>South Projection Factor</t>
   </si>
   <si>
-    <t>1.8.0</t>
-  </si>
-  <si>
     <t>AWS Tag</t>
   </si>
   <si>
@@ -2325,7 +2322,10 @@
     <t>Overhangs PF East</t>
   </si>
   <si>
-    <t>0.3.7</t>
+    <t>1.9.0</t>
+  </si>
+  <si>
+    <t>0.4.0</t>
   </si>
 </sst>
 </file>
@@ -2487,8 +2487,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1559">
+  <cellStyleXfs count="1561">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4150,7 +4152,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1559">
+  <cellStyles count="1561">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4930,6 +4932,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1554" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1556" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1560" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5709,6 +5712,7 @@
     <cellStyle name="Hyperlink" xfId="1553" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1555" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1559" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6010,7 +6014,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -6069,7 +6075,7 @@
         <v>471</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>730</v>
+        <v>760</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>618</v>
@@ -6153,16 +6159,16 @@
     </row>
     <row r="10" spans="1:6" s="23" customFormat="1" ht="28">
       <c r="A10" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>731</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>732</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1">
@@ -6322,14 +6328,14 @@
       </c>
       <c r="B26" s="18">
         <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="C26" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B22,Lookups!$A$21:$A$27,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D26" s="27">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="E26" s="23"/>
     </row>
@@ -6555,34 +6561,34 @@
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" ht="56">
       <c r="A46" s="6" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="19"/>
       <c r="F46" s="8" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="2" customFormat="1">
       <c r="A47" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="B47" s="25" t="s">
         <v>751</v>
       </c>
-      <c r="B47" s="25" t="s">
-        <v>752</v>
-      </c>
       <c r="C47" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="25"/>
       <c r="F47" s="7" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="23" customFormat="1">
@@ -6591,18 +6597,18 @@
     </row>
     <row r="49" spans="1:6" s="2" customFormat="1" ht="42">
       <c r="A49" s="6" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
       <c r="F49" s="8" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
   </sheetData>
@@ -7705,7 +7711,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C26" s="39" t="s">
         <v>76</v>
@@ -7869,7 +7875,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C30" s="39" t="s">
         <v>76</v>
@@ -7909,7 +7915,7 @@
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="46" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>77</v>
@@ -8033,7 +8039,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C34" s="39" t="s">
         <v>76</v>
@@ -8197,7 +8203,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C38" s="39" t="s">
         <v>170</v>
@@ -8243,7 +8249,7 @@
         <v>172</v>
       </c>
       <c r="F39" s="42" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="G39" s="42" t="s">
         <v>64</v>
@@ -8401,7 +8407,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C43" s="39" t="s">
         <v>170</v>
@@ -8441,13 +8447,13 @@
       </c>
       <c r="C44" s="42"/>
       <c r="D44" s="42" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E44" s="42" t="s">
         <v>172</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="G44" s="42" t="s">
         <v>64</v>
@@ -19410,7 +19416,7 @@
         <v>658</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="22" customFormat="1">
@@ -19427,7 +19433,7 @@
         <v>656</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1">
@@ -19444,7 +19450,7 @@
         <v>657</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="22" customFormat="1">
@@ -19461,7 +19467,7 @@
         <v>659</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -19478,21 +19484,21 @@
         <v>661</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1">
       <c r="A11" s="29" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>446</v>
       </c>
       <c r="C11" s="22" t="s">
+        <v>737</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>738</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>739</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>664</v>
@@ -19500,16 +19506,16 @@
     </row>
     <row r="12" spans="1:7" s="22" customFormat="1">
       <c r="A12" s="29" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>447</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>664</v>

</xml_diff>

<commit_message>
update to 1.9.3 for openstudio 1.6 support
</commit_message>
<xml_diff>
--- a/projects/template_lhs_discrete_continuous.xlsx
+++ b/projects/template_lhs_discrete_continuous.xlsx
@@ -2322,10 +2322,10 @@
     <t>Overhangs PF East</t>
   </si>
   <si>
-    <t>1.9.0</t>
-  </si>
-  <si>
     <t>0.4.0</t>
+  </si>
+  <si>
+    <t>1.9.3</t>
   </si>
 </sst>
 </file>
@@ -6015,7 +6015,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6053,7 +6053,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>437</v>
@@ -6075,7 +6075,7 @@
         <v>471</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>618</v>

</xml_diff>